<commit_message>
owner pdf link send to the client
</commit_message>
<xml_diff>
--- a/resources/hiring.xlsx
+++ b/resources/hiring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Techidol solutions\CRM\crm_dashboard\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7A23B6-E6F6-4D87-87A7-95CD923C1BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8D0D5A-53FC-4E9D-9277-BFC8F927E35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -586,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView tabSelected="1" topLeftCell="H34" workbookViewId="0">
+      <selection activeCell="U39" sqref="U39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -693,7 +693,7 @@
         <v>31</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2">
         <v>31</v>
@@ -793,7 +793,7 @@
         <v>31</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M4">
         <v>31</v>
@@ -843,7 +843,7 @@
         <v>31</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M5">
         <v>31</v>
@@ -1043,7 +1043,7 @@
         <v>31</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M9">
         <v>31</v>
@@ -1093,7 +1093,7 @@
         <v>31</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M10">
         <v>31</v>
@@ -1143,7 +1143,7 @@
         <v>31</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M11">
         <v>31</v>
@@ -1193,7 +1193,7 @@
         <v>31</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12">
         <v>31</v>
@@ -1243,7 +1243,7 @@
         <v>31</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M13">
         <v>31</v>
@@ -1443,7 +1443,7 @@
         <v>31</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M17">
         <v>31</v>
@@ -1493,7 +1493,7 @@
         <v>31</v>
       </c>
       <c r="L18">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M18">
         <v>31</v>
@@ -1643,7 +1643,7 @@
         <v>31</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M21">
         <v>31</v>
@@ -1793,7 +1793,7 @@
         <v>31</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M24">
         <v>31</v>
@@ -1893,7 +1893,7 @@
         <v>31</v>
       </c>
       <c r="L26">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M26">
         <v>31</v>
@@ -1993,7 +1993,7 @@
         <v>31</v>
       </c>
       <c r="L28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M28">
         <v>31</v>
@@ -2143,7 +2143,7 @@
         <v>31</v>
       </c>
       <c r="L31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M31">
         <v>31</v>
@@ -2343,7 +2343,7 @@
         <v>31</v>
       </c>
       <c r="L35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M35">
         <v>31</v>
@@ -2493,7 +2493,7 @@
         <v>31</v>
       </c>
       <c r="L38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M38">
         <v>31</v>
@@ -2593,7 +2593,7 @@
         <v>31</v>
       </c>
       <c r="L40">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M40">
         <v>31</v>

</xml_diff>